<commit_message>
columna IMPORTE simulador XLS
</commit_message>
<xml_diff>
--- a/public/assets/plantillas_excel/Mod_09/SIZ_simulador.xlsx
+++ b/public/assets/plantillas_excel/Mod_09/SIZ_simulador.xlsx
@@ -8,24 +8,35 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\siz_p\public\assets\plantillas_excel\Mod_09\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D42AF14E-B1A5-437A-9068-5FBB95BB862D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F4F2BEA-2B07-4EF3-95A0-198045AEC88C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="15600" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="15600" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RESUMEN" sheetId="1" r:id="rId1"/>
     <sheet name="DETALLE" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">DETALLE!$A$5:$P$5</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">DETALLE!$A$5:$Q$5</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">RESUMEN!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="54">
   <si>
     <t>SALOTTO, S.A. DE C.V.</t>
   </si>
@@ -184,6 +195,9 @@
   </si>
   <si>
     <t>DESCRIPCION_ORIGEN</t>
+  </si>
+  <si>
+    <t>IMPORTE MXP</t>
   </si>
 </sst>
 </file>
@@ -297,7 +311,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -338,6 +352,18 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -396,7 +422,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="167" fontId="6" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -437,23 +463,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="165" fontId="4" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -465,6 +474,24 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="166" fontId="12" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="1" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -941,7 +968,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AI780"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="C1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
@@ -968,26 +995,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:35" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
       <c r="K1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="L1" s="25"/>
-      <c r="M1" s="25"/>
-      <c r="N1" s="25"/>
-      <c r="O1" s="25"/>
-      <c r="P1" s="25"/>
-      <c r="Q1" s="25"/>
-      <c r="R1" s="25"/>
-      <c r="S1" s="25"/>
-      <c r="T1" s="25"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="18"/>
+      <c r="N1" s="18"/>
+      <c r="O1" s="18"/>
+      <c r="P1" s="18"/>
+      <c r="Q1" s="18"/>
+      <c r="R1" s="18"/>
+      <c r="S1" s="18"/>
+      <c r="T1" s="18"/>
       <c r="U1" s="1"/>
       <c r="V1" s="1"/>
       <c r="W1" s="1"/>
@@ -1005,26 +1032,26 @@
       <c r="AI1" s="1"/>
     </row>
     <row r="2" spans="1:35" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="I2" s="26"/>
-      <c r="J2" s="26"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
       <c r="K2" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="L2" s="26"/>
-      <c r="M2" s="26"/>
-      <c r="N2" s="26"/>
-      <c r="O2" s="26"/>
-      <c r="P2" s="26"/>
-      <c r="Q2" s="26"/>
-      <c r="R2" s="26"/>
-      <c r="S2" s="26"/>
-      <c r="T2" s="26"/>
+      <c r="L2" s="19"/>
+      <c r="M2" s="19"/>
+      <c r="N2" s="19"/>
+      <c r="O2" s="19"/>
+      <c r="P2" s="19"/>
+      <c r="Q2" s="19"/>
+      <c r="R2" s="19"/>
+      <c r="S2" s="19"/>
+      <c r="T2" s="19"/>
       <c r="U2" s="1"/>
       <c r="V2" s="1"/>
       <c r="W2" s="1"/>
@@ -1042,26 +1069,26 @@
       <c r="AI2" s="1"/>
     </row>
     <row r="3" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="27"/>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="27"/>
-      <c r="I3" s="27"/>
-      <c r="J3" s="27"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+      <c r="I3" s="20"/>
+      <c r="J3" s="20"/>
       <c r="K3" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="L3" s="27"/>
-      <c r="M3" s="27"/>
-      <c r="N3" s="27"/>
-      <c r="O3" s="27"/>
-      <c r="P3" s="27"/>
-      <c r="Q3" s="27"/>
-      <c r="R3" s="27"/>
-      <c r="S3" s="27"/>
-      <c r="T3" s="27"/>
+      <c r="L3" s="20"/>
+      <c r="M3" s="20"/>
+      <c r="N3" s="20"/>
+      <c r="O3" s="20"/>
+      <c r="P3" s="20"/>
+      <c r="Q3" s="20"/>
+      <c r="R3" s="20"/>
+      <c r="S3" s="20"/>
+      <c r="T3" s="20"/>
       <c r="U3" s="1"/>
       <c r="V3" s="1"/>
       <c r="W3" s="1"/>
@@ -1090,11 +1117,11 @@
       <c r="E4" s="6"/>
       <c r="G4" s="6"/>
       <c r="H4" s="6"/>
-      <c r="J4" s="29" t="s">
+      <c r="J4" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="K4" s="28"/>
-      <c r="L4" s="28"/>
+      <c r="K4" s="21"/>
+      <c r="L4" s="21"/>
       <c r="M4" s="2"/>
       <c r="O4" s="6"/>
       <c r="P4" s="7"/>
@@ -1138,14 +1165,14 @@
     </row>
     <row r="7" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="8" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="18" t="s">
+      <c r="A8" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
+      <c r="B8" s="23"/>
+      <c r="C8" s="23"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="23"/>
     </row>
     <row r="9" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="16" t="s">
@@ -2041,11 +2068,11 @@
     <tabColor rgb="FF7030A0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:P966"/>
+  <dimension ref="A1:Q966"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F12" sqref="F12"/>
+      <selection pane="bottomLeft" activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2057,37 +2084,81 @@
     <col min="5" max="5" width="15.85546875" customWidth="1"/>
     <col min="6" max="6" width="29.85546875" customWidth="1"/>
     <col min="10" max="10" width="15.140625" customWidth="1"/>
-    <col min="11" max="11" width="19.140625" customWidth="1"/>
-    <col min="12" max="12" width="19.42578125" customWidth="1"/>
-    <col min="14" max="14" width="22.140625" customWidth="1"/>
-    <col min="15" max="15" width="22.85546875" customWidth="1"/>
-    <col min="16" max="16" width="19.140625" customWidth="1"/>
+    <col min="11" max="12" width="19.140625" customWidth="1"/>
+    <col min="13" max="13" width="19.42578125" customWidth="1"/>
+    <col min="15" max="15" width="22.140625" customWidth="1"/>
+    <col min="16" max="16" width="22.85546875" customWidth="1"/>
+    <col min="17" max="17" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="19" t="s">
+    <row r="1" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="21"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
+      <c r="L1" s="27"/>
+      <c r="M1" s="27"/>
     </row>
-    <row r="2" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="19"/>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="21"/>
+    <row r="2" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A2" s="24"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="27"/>
+      <c r="J2" s="27"/>
+      <c r="K2" s="27"/>
+      <c r="L2" s="27"/>
+      <c r="M2" s="27"/>
     </row>
-    <row r="3" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="22" t="s">
+    <row r="3" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="B3" s="23"/>
-      <c r="C3" s="23"/>
-      <c r="D3" s="24"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="27"/>
+      <c r="H3" s="27"/>
+      <c r="I3" s="27"/>
+      <c r="J3" s="27"/>
+      <c r="K3" s="27"/>
+      <c r="L3" s="27"/>
+      <c r="M3" s="27"/>
     </row>
-    <row r="4" spans="1:16" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="5" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A4" s="27"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="27"/>
+      <c r="K4" s="27"/>
+      <c r="L4" s="27">
+        <f>SUBTOTAL(9,L6:L2000)</f>
+        <v>0</v>
+      </c>
+      <c r="M4" s="27"/>
+    </row>
+    <row r="5" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>4</v>
       </c>
@@ -2122,32 +2193,35 @@
         <v>45</v>
       </c>
       <c r="L5" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="M5" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="M5" s="11" t="s">
+      <c r="N5" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="N5" s="11" t="s">
+      <c r="O5" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="O5" s="11" t="s">
+      <c r="P5" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="P5" s="11" t="s">
+      <c r="Q5" s="11" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="7" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="8" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="9" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="10" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="11" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="12" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="13" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="14" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="15" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="16" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="6" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="7" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="8" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="9" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="10" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="11" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="12" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="13" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="16" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3099,7 +3173,7 @@
     <row r="965" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="966" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <autoFilter ref="A5:P5" xr:uid="{00000000-0001-0000-0100-000000000000}"/>
+  <autoFilter ref="A5:Q5" xr:uid="{00000000-0001-0000-0100-000000000000}"/>
   <mergeCells count="3">
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A2:D2"/>

</xml_diff>